<commit_message>
changes from new machine
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinaj\Eclipse Project\OpsVedaAutomation\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7F2BA9-4BC4-4584-9A2F-C5DD94D88AE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8F25CC70-33A1-4247-AD20-24CF3FCA3FBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AA6705C7-D248-4EC0-83F8-9014E5C20A31}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20760" windowHeight="11820" xr2:uid="{AA6705C7-D248-4EC0-83F8-9014E5C20A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Browser setting URL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -434,10 +430,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>